<commit_message>
updating FAD numbers and survey data, adding table/figure files
</commit_message>
<xml_diff>
--- a/raw_data/survey/mgmt_table.xlsx
+++ b/raw_data/survey/mgmt_table.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/github/kuni_fads/raw_data/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD73CA59-74F3-D142-B02D-7F1B252402B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380EF01E-0449-514A-83F5-6E4FF79DD0FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="460" windowWidth="13240" windowHeight="13680" xr2:uid="{0FCB2853-2D9F-E049-8B03-8BFDD79293AA}"/>
+    <workbookView xWindow="10020" yWindow="460" windowWidth="13240" windowHeight="13680" xr2:uid="{0FCB2853-2D9F-E049-8B03-8BFDD79293AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
   <si>
     <t>Antigua and Barbuda</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Cayman Islands</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -752,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E1BAA-A661-7B43-BB8E-90A80EC2E121}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="3"/>

</xml_diff>

<commit_message>
updating guadeloupe survey responses
</commit_message>
<xml_diff>
--- a/raw_data/survey/mgmt_table.xlsx
+++ b/raw_data/survey/mgmt_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/github/kuni_fads/raw_data/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380EF01E-0449-514A-83F5-6E4FF79DD0FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC961A6F-AFEE-0F48-AECA-BCCEDF0E6954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="460" windowWidth="13240" windowHeight="13680" xr2:uid="{0FCB2853-2D9F-E049-8B03-8BFDD79293AA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>Antigua and Barbuda</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -750,7 +753,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,7 +1144,9 @@
       <c r="J15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="L15" s="6"/>
       <c r="M15" s="3"/>
       <c r="N15" s="1"/>

</xml_diff>